<commit_message>
Gantt i Dokumentacja Projektu
Zaaktualizowany harmonogram Gantta i utworzony szablon dokumentacji projektu
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semestr 4\projekt inżynierski\870ziemianski\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studia\UR\Nauka\SEMESTR VI\Programowanie Zespołowe Szczur\Projekt System Do Zarządzania\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,39 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Projekt wykresu Gannta</t>
-  </si>
-  <si>
-    <t>Projekt przypadków użycia</t>
-  </si>
-  <si>
-    <t>Implementacja Ontologii</t>
-  </si>
-  <si>
-    <t>Implementacja Graficznego Interfejsu Użytkownika</t>
-  </si>
-  <si>
-    <t>Zaimplementowanie parsera</t>
-  </si>
-  <si>
-    <t>Implementacja generatora</t>
-  </si>
-  <si>
-    <t>Implementacja struktury projektu</t>
-  </si>
-  <si>
-    <t>Poprawienie Ontologi</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Poczatek</t>
   </si>
   <si>
     <t>Zadanie</t>
-  </si>
-  <si>
-    <t>Zbieranie danych z zakresu Motoryzacji</t>
   </si>
   <si>
     <t>Trwanie</t>
@@ -67,11 +40,29 @@
   <si>
     <t>Nr</t>
   </si>
+  <si>
+    <t xml:space="preserve"> Opracowanie wizji projektu i przygotowanie środowiska pracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Działające okna (zakładki) min. 2 modułów (bez bazy danych)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">działająca i wypełniana automatycznie baza danych </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> podłączenie bazy danych do istniejących okienek </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> stworzenie biblioteki generującej raporty w PDF i uruchomienie brakujących modułów</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wykonanie brakujących elementów (testów, javadoc, itd.) oraz instalatora</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-415]d\ mmm;@"/>
   </numFmts>
@@ -84,7 +75,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,18 +84,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -113,207 +98,33 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -334,7 +145,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
   <c:roundedCorners val="0"/>
@@ -385,76 +196,58 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$3:$C$11</c:f>
+              <c:f>Arkusz1!$C$3:$C$8</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Projekt wykresu Gannta</c:v>
+                  <c:v> Opracowanie wizji projektu i przygotowanie środowiska pracy</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Projekt przypadków użycia</c:v>
+                  <c:v> Działające okna (zakładki) min. 2 modułów (bez bazy danych)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Implementacja Ontologii</c:v>
+                  <c:v>działająca i wypełniana automatycznie baza danych </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Zbieranie danych z zakresu Motoryzacji</c:v>
+                  <c:v> podłączenie bazy danych do istniejących okienek </c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Poprawienie Ontologi</c:v>
+                  <c:v> stworzenie biblioteki generującej raporty w PDF i uruchomienie brakujących modułów</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Implementacja struktury projektu</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Zaimplementowanie parsera</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Implementacja generatora</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Implementacja Graficznego Interfejsu Użytkownika</c:v>
+                  <c:v> wykonanie brakujących elementów (testów, javadoc, itd.) oraz instalatora</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$D$3:$D$11</c:f>
+              <c:f>Arkusz1!$D$3:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>[$-415]d\ mmm;@</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42849</c:v>
+                  <c:v>43160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42850</c:v>
+                  <c:v>43174</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42853</c:v>
+                  <c:v>43195</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42855</c:v>
+                  <c:v>43209</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42856</c:v>
+                  <c:v>43230</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42858</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42868</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>42873</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>42880</c:v>
+                  <c:v>43244</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000B-3854-4DC2-A9CD-1226EFAB8C9E}"/>
             </c:ext>
@@ -476,7 +269,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="00B050"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -500,76 +295,58 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$C$3:$C$11</c:f>
+              <c:f>Arkusz1!$C$3:$C$8</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Projekt wykresu Gannta</c:v>
+                  <c:v> Opracowanie wizji projektu i przygotowanie środowiska pracy</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Projekt przypadków użycia</c:v>
+                  <c:v> Działające okna (zakładki) min. 2 modułów (bez bazy danych)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Implementacja Ontologii</c:v>
+                  <c:v>działająca i wypełniana automatycznie baza danych </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Zbieranie danych z zakresu Motoryzacji</c:v>
+                  <c:v> podłączenie bazy danych do istniejących okienek </c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Poprawienie Ontologi</c:v>
+                  <c:v> stworzenie biblioteki generującej raporty w PDF i uruchomienie brakujących modułów</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Implementacja struktury projektu</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Zaimplementowanie parsera</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Implementacja generatora</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Implementacja Graficznego Interfejsu Użytkownika</c:v>
+                  <c:v> wykonanie brakujących elementów (testów, javadoc, itd.) oraz instalatora</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$E$3:$E$11</c:f>
+              <c:f>Arkusz1!$E$3:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-3854-4DC2-A9CD-1226EFAB8C9E}"/>
             </c:ext>
@@ -586,11 +363,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="387476424"/>
-        <c:axId val="387474784"/>
+        <c:axId val="1458069680"/>
+        <c:axId val="1458071312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="387476424"/>
+        <c:axId val="1458069680"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -619,6 +396,9 @@
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln w="0">
+                  <a:noFill/>
+                </a:ln>
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -630,10 +410,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387474784"/>
+        <c:crossAx val="1458071312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -641,11 +421,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="387474784"/>
+        <c:axId val="1458071312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="42885"/>
-          <c:min val="42849"/>
+          <c:min val="43150"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -690,13 +469,13 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387476424"/>
+        <c:crossAx val="1458069680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="2"/>
+        <c:majorUnit val="5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -732,7 +511,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pl-PL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1321,13 +1100,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>600073</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>68716</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1335,7 +1114,7 @@
         <xdr:cNvPr id="4" name="Wykres 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A652F57-9DD4-4B19-AEAC-7B18118BB9D6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A652F57-9DD4-4B19-AEAC-7B18118BB9D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1653,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F11"/>
+  <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,192 +1447,128 @@
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>13</v>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="16">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8">
-        <v>42849</v>
-      </c>
-      <c r="E3" s="12">
-        <v>1</v>
-      </c>
-      <c r="F3" s="9">
-        <f>D3+E3</f>
-        <v>42850</v>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>43160</v>
+      </c>
+      <c r="E3" s="1">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3">
+        <v>43174</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="15">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10">
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3">
         <f>F3</f>
-        <v>42850</v>
-      </c>
-      <c r="E4" s="13">
-        <v>3</v>
-      </c>
-      <c r="F4" s="6">
-        <f t="shared" ref="F4:F11" si="0">D4+E4</f>
-        <v>42853</v>
+        <v>43174</v>
+      </c>
+      <c r="E4" s="1">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3">
+        <v>43195</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="15">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3">
         <f>F4</f>
-        <v>42853</v>
-      </c>
-      <c r="E5" s="13">
-        <v>2</v>
-      </c>
-      <c r="F5" s="6">
-        <f t="shared" si="0"/>
-        <v>42855</v>
+        <v>43195</v>
+      </c>
+      <c r="E5" s="1">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3">
+        <v>43209</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="15">
+      <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="10">
-        <f t="shared" ref="D5:D11" si="1">F5</f>
-        <v>42855</v>
-      </c>
-      <c r="E6" s="13">
-        <v>1</v>
-      </c>
-      <c r="F6" s="6">
-        <f t="shared" si="0"/>
-        <v>42856</v>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3">
+        <f>F5</f>
+        <v>43209</v>
+      </c>
+      <c r="E6" s="1">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3">
+        <v>43230</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="15">
+      <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3">
         <f>F6</f>
-        <v>42856</v>
-      </c>
-      <c r="E7" s="13">
-        <v>2</v>
-      </c>
-      <c r="F7" s="6">
-        <f t="shared" si="0"/>
-        <v>42858</v>
+        <v>43230</v>
+      </c>
+      <c r="E7" s="1">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3">
+        <v>43244</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
+      <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="10">
-        <f t="shared" si="1"/>
-        <v>42858</v>
-      </c>
-      <c r="E8" s="13">
+      <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="6">
-        <f t="shared" si="0"/>
-        <v>42868</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="15">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="10">
-        <f t="shared" si="1"/>
-        <v>42868</v>
-      </c>
-      <c r="E9" s="13">
-        <v>5</v>
-      </c>
-      <c r="F9" s="6">
-        <f t="shared" si="0"/>
-        <v>42873</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="15">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="10">
-        <f>F9</f>
-        <v>42873</v>
-      </c>
-      <c r="E10" s="13">
-        <v>7</v>
-      </c>
-      <c r="F10" s="6">
-        <f t="shared" si="0"/>
-        <v>42880</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="17">
-        <v>9</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="11">
-        <f>F10</f>
-        <v>42880</v>
-      </c>
-      <c r="E11" s="14">
-        <v>4</v>
-      </c>
-      <c r="F11" s="7">
-        <f t="shared" si="0"/>
-        <v>42884</v>
+      <c r="D8" s="3">
+        <f t="shared" ref="D6:D8" si="0">F7</f>
+        <v>43244</v>
+      </c>
+      <c r="E8" s="1">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3">
+        <v>43258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>